<commit_message>
New data and data breakdowns
</commit_message>
<xml_diff>
--- a/Assignment1/data-import.xlsx
+++ b/Assignment1/data-import.xlsx
@@ -4,21 +4,46 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="345" windowWidth="28605" windowHeight="12630" activeTab="1"/>
+    <workbookView xWindow="-300" yWindow="345" windowWidth="28605" windowHeight="12630" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1. Create Structure" sheetId="4" r:id="rId1"/>
     <sheet name="2. Create Data" sheetId="6" r:id="rId2"/>
+    <sheet name="Facilities vs Years" sheetId="10" r:id="rId3"/>
+    <sheet name="Designs vs Years" sheetId="11" r:id="rId4"/>
+    <sheet name="Price vs Calories" sheetId="12" r:id="rId5"/>
+    <sheet name="Suppliers vs Years" sheetId="13" r:id="rId6"/>
+    <sheet name="Country vs Sales Periods" sheetId="14" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_paloimportactive">FALSE</definedName>
+    <definedName name="_palopasteviewcolwidth" localSheetId="6">14</definedName>
+    <definedName name="_palopasteviewcolwidth" localSheetId="3">14</definedName>
+    <definedName name="_palopasteviewcolwidth" localSheetId="2">14</definedName>
+    <definedName name="_palopasteviewcolwidth" localSheetId="4">14</definedName>
+    <definedName name="_palopasteviewcolwidth" localSheetId="5">14</definedName>
+    <definedName name="_palopasteviewident" localSheetId="6">TRUE</definedName>
+    <definedName name="_palopasteviewident" localSheetId="3">TRUE</definedName>
+    <definedName name="_palopasteviewident" localSheetId="2">TRUE</definedName>
+    <definedName name="_palopasteviewident" localSheetId="4">TRUE</definedName>
+    <definedName name="_palopasteviewident" localSheetId="5">TRUE</definedName>
+    <definedName name="_palopasteviewzerosuppression" localSheetId="6">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppression" localSheetId="3">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppression" localSheetId="2">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppression" localSheetId="4">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppression" localSheetId="5">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppressionalsocalculatednull" localSheetId="6">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppressionalsocalculatednull" localSheetId="3">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppressionalsocalculatednull" localSheetId="2">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppressionalsocalculatednull" localSheetId="4">FALSE</definedName>
+    <definedName name="_palopasteviewzerosuppressionalsocalculatednull" localSheetId="5">FALSE</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
   <si>
     <t>localhost/BurgerStore</t>
   </si>
@@ -74,9 +99,6 @@
     <t>↑ ComboCalories</t>
   </si>
   <si>
-    <t>Combos Attribute Dimension</t>
-  </si>
-  <si>
     <t>← Add store to elements</t>
   </si>
   <si>
@@ -110,12 +132,6 @@
     <t>← Conversions</t>
   </si>
   <si>
-    <t>Calories Attribute Name</t>
-  </si>
-  <si>
-    <t>Calories</t>
-  </si>
-  <si>
     <t>Cube Name</t>
   </si>
   <si>
@@ -149,18 +165,12 @@
     <t>← Add country to "All Stores"</t>
   </si>
   <si>
-    <t>(with Calories attribute)</t>
-  </si>
-  <si>
     <t>Warning: Magic</t>
   </si>
   <si>
     <t>← Add number of sales dimension</t>
   </si>
   <si>
-    <t>← Add calories attribute to combo</t>
-  </si>
-  <si>
     <t>Required Dimensions (in cube in this order)</t>
   </si>
   <si>
@@ -195,6 +205,63 @@
   </si>
   <si>
     <t>Not Used</t>
+  </si>
+  <si>
+    <t>PriceRange</t>
+  </si>
+  <si>
+    <t>PriceRange creation</t>
+  </si>
+  <si>
+    <t>$2 - $3.99</t>
+  </si>
+  <si>
+    <t>$0 - $1.99</t>
+  </si>
+  <si>
+    <t>$4 - $5.99</t>
+  </si>
+  <si>
+    <t>$6 - $7.99</t>
+  </si>
+  <si>
+    <t>$8 - $9.99</t>
+  </si>
+  <si>
+    <t>$10+</t>
+  </si>
+  <si>
+    <t>← Make "All Prices"</t>
+  </si>
+  <si>
+    <t>0 - 249</t>
+  </si>
+  <si>
+    <t>250 - 499</t>
+  </si>
+  <si>
+    <t>500 - 749</t>
+  </si>
+  <si>
+    <t>750 - 999</t>
+  </si>
+  <si>
+    <t>1000 - 1249</t>
+  </si>
+  <si>
+    <t>1250 - 1499</t>
+  </si>
+  <si>
+    <t>1500+</t>
+  </si>
+  <si>
+    <t>CalorieRange creation</t>
+  </si>
+  <si>
+    <t>CalorieRange</t>
+  </si>
+  <si>
+    <t>← Make "Any Calories"</t>
   </si>
 </sst>
 </file>
@@ -204,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -376,6 +443,12 @@
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -827,7 +900,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="49" fontId="20" fillId="38" borderId="0" xfId="47">
@@ -840,6 +913,20 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="37"/>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="44" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="29" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="32" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="39" borderId="10" xfId="43"/>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" xfId="29" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="___col1" xfId="29"/>
@@ -1270,10 +1357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1394,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1332,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="e">
-        <f>VLOOKUP($F$1,$D$21:$E$32,2)</f>
+        <f>VLOOKUP($F$1,$D$21:$E$26,2)</f>
         <v>#N/A</v>
       </c>
       <c r="G2" s="1">
@@ -1351,7 +1438,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1371,7 +1458,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>13</v>
@@ -1383,13 +1470,13 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1410,11 +1497,11 @@
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E8" s="7"/>
       <c r="G8" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1429,7 +1516,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1442,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1455,12 +1542,12 @@
         <v>0</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="D12" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E12" s="7"/>
       <c r="G12" s="5" t="b">
@@ -1468,12 +1555,12 @@
         <v>0</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -1482,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1495,22 +1582,20 @@
         <v>0</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="E15" s="7"/>
       <c r="G15" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$15,"c","All Combos")</f>
         <v>0</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1523,20 +1608,26 @@
         <v>0</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="G18" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$9,"c",$B$2,"All Stores",1)</f>
         <v>0</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1545,7 +1636,7 @@
     </row>
     <row r="20" spans="4:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3"/>
       <c r="G20" s="5" t="b">
@@ -1553,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1561,14 +1652,14 @@
         <v>1</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G21" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$10,"n",$C$2,"All Designs",1)</f>
         <v>0</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1576,14 +1667,14 @@
         <v>2</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G22" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$11,"n",$D$2,"Any Facilities", 1)</f>
         <v>0</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1591,14 +1682,14 @@
         <v>3</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G23" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$13,"n",$F$2,"All Periods",1)</f>
         <v>0</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1606,14 +1697,14 @@
         <v>4</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G24" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$14,"n",$G$2,"All Years",1)</f>
         <v>0</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1621,14 +1712,14 @@
         <v>5</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G25" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$12,"n",$E$2,"All Periods",1)</f>
         <v>0</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1636,14 +1727,14 @@
         <v>6</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G26" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$15,"n",$H$2,"All Combos",1)</f>
         <v>0</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1653,31 +1744,237 @@
         <v>0</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E29" s="7"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"c","All Prices")</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="30" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E30" s="7"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="D30">
+        <v>200</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$29,"All Prices", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="31" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="E31" s="7"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E32" s="7"/>
+      <c r="D31">
+        <v>400</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$30,"All Prices", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>600</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G32" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$31,"All Prices", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>800</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$32,"All Prices", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$33,"All Prices", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G35" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$34,"All Prices", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$18,"c","Any Calories")</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>250</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$37,"Any Calories", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>500</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$38,"Any Calories", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>750</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G40" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$39,"Any Calories", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>1000</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$40,"Any Calories", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>1250</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$41,"Any Calories", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>1500</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$42,"Any Calories", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G44" s="5" t="b">
+        <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$43,"Any Calories", 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1687,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1724,7 +2021,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1746,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="e">
-        <f>VLOOKUP($F$1,$D$21:$E$32,2)</f>
+        <f>VLOOKUP($F$1,$D$21:$E$26,2)</f>
         <v>#N/A</v>
       </c>
       <c r="G2" s="1">
@@ -1761,20 +2058,20 @@
         <f>$I$1</f>
         <v>0</v>
       </c>
-      <c r="J2" s="1">
-        <f>$J$1</f>
-        <v>0</v>
+      <c r="J2" s="1" t="str">
+        <f>VLOOKUP($J$1,$D$37:$E$43,2,TRUE)</f>
+        <v>0 - 249</v>
       </c>
       <c r="K2" s="1">
         <f>$K$1</f>
         <v>0</v>
       </c>
-      <c r="L2" s="1">
-        <f>$L$1/100</f>
-        <v>0</v>
+      <c r="L2" s="1" t="str">
+        <f>VLOOKUP($L$1,$D$29:$E$34,2,TRUE)</f>
+        <v>$0 - $1.99</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1782,7 +2079,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -1794,7 +2091,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>13</v>
@@ -1809,10 +2106,10 @@
         <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1830,214 +2127,1241 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="7" t="str">
-        <f>"#_"&amp;$D$15</f>
-        <v>#_Combos</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E8" s="7"/>
       <c r="G8" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
       <c r="D9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="G9" s="5">
-        <f ca="1">_xll.PALO.SETDATA($J$2,FALSE,$B$7,$B$8,$B$9,$H$2)</f>
-        <v>0</v>
+      <c r="G9" s="5" t="e">
+        <f ca="1">_xll.PALO.SETDATA($K$2,FALSE,$B$7,$B$10,$A$2,$C$2,$D$2,$E$2,$F$2,$G$2,$H$2,$I$2,$L$2,$J$2)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="G10" s="5" t="e">
-        <f ca="1">_xll.PALO.SETDATA($K$2,FALSE,$B$7,$B$10,$A$2,$C$2,$D$2,$E$2,$F$2,$G$2,$H$2,$I$2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D12" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D13" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D16" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23">
         <v>3</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24">
         <v>4</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25">
         <v>5</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26">
         <v>6</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E27" s="7"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="4:8" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E28" s="7"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E32" s="7"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>200</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>400</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>600</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>800</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>250</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>500</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>750</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>1000</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>1250</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>1500</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Stores","All Stores",1,"")</f>
+        <v>All Stores</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Designs","All Designs",1,"")</f>
+        <v>All Designs</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"SalesPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PromotionalPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Combos","All Combos",1,"")</f>
+        <v>All Combos</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Suppliers","All Suppliers",1,"")</f>
+        <v>All Suppliers</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","All Prices",1,"")</f>
+        <v>All Prices</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","Any Calories",1,"")</f>
+        <v>Any Calories</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Facilities","Dine-in",0,"Any Facilities\Dine-in")</f>
+        <v>Dine-in</v>
+      </c>
+      <c r="C12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Facilities","Drive-through",0,"Any Facilities\Drive-through")</f>
+        <v>Drive-through</v>
+      </c>
+      <c r="D12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Facilities","Both",0,"Any Facilities\Both")</f>
+        <v>Both</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2008",0,"All Years\2008")</f>
+        <v>2008</v>
+      </c>
+      <c r="B13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,B$12,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3278289</v>
+      </c>
+      <c r="C13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,C$12,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3260388</v>
+      </c>
+      <c r="D13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,D$12,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>2082676</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2009",0,"All Years\2009")</f>
+        <v>2009</v>
+      </c>
+      <c r="B14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,B$12,$A$5,$A$6,$A14,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3379143</v>
+      </c>
+      <c r="C14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,C$12,$A$5,$A$6,$A14,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3319011</v>
+      </c>
+      <c r="D14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,D$12,$A$5,$A$6,$A14,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>2194353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2010",0,"All Years\2010")</f>
+        <v>2010</v>
+      </c>
+      <c r="B15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,B$12,$A$5,$A$6,$A15,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3362891</v>
+      </c>
+      <c r="C15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,C$12,$A$5,$A$6,$A15,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3278076</v>
+      </c>
+      <c r="D15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,D$12,$A$5,$A$6,$A15,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>2213186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2011",0,"All Years\2011")</f>
+        <v>2011</v>
+      </c>
+      <c r="B16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,B$12,$A$5,$A$6,$A16,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3331692</v>
+      </c>
+      <c r="C16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,C$12,$A$5,$A$6,$A16,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3329445</v>
+      </c>
+      <c r="D16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,D$12,$A$5,$A$6,$A16,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>2204859</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2012",0,"All Years\2012")</f>
+        <v>2012</v>
+      </c>
+      <c r="B17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,B$12,$A$5,$A$6,$A17,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>563618</v>
+      </c>
+      <c r="C17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,C$12,$A$5,$A$6,$A17,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>559616</v>
+      </c>
+      <c r="D17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,D$12,$A$5,$A$6,$A17,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>371054</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Stores","All Stores",1,"")</f>
+        <v>All Stores</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Facilities","Any Facilities",1,"")</f>
+        <v>Any Facilities</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"SalesPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PromotionalPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Combos","All Combos",1,"")</f>
+        <v>All Combos</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Suppliers","All Suppliers",1,"")</f>
+        <v>All Suppliers</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","All Prices",1,"")</f>
+        <v>All Prices</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","Any Calories",1,"")</f>
+        <v>Any Calories</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Designs","Avant-garde",0,"All Designs\Avant-garde")</f>
+        <v>Avant-garde</v>
+      </c>
+      <c r="C12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Designs","No roof",0,"All Designs\No roof")</f>
+        <v>No roof</v>
+      </c>
+      <c r="D12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Designs","Upside-down",0,"All Designs\Upside-down")</f>
+        <v>Upside-down</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2008",0,"All Years\2008")</f>
+        <v>2008</v>
+      </c>
+      <c r="B13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,B$12,$A$4,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3875214</v>
+      </c>
+      <c r="C13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,C$12,$A$4,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3624583</v>
+      </c>
+      <c r="D13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,D$12,$A$4,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>1121556</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2009",0,"All Years\2009")</f>
+        <v>2009</v>
+      </c>
+      <c r="B14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,B$12,$A$4,$A$5,$A$6,$A14,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3959781</v>
+      </c>
+      <c r="C14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,C$12,$A$4,$A$5,$A$6,$A14,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3794831</v>
+      </c>
+      <c r="D14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,D$12,$A$4,$A$5,$A$6,$A14,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>1137895</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2010",0,"All Years\2010")</f>
+        <v>2010</v>
+      </c>
+      <c r="B15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,B$12,$A$4,$A$5,$A$6,$A15,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3906224</v>
+      </c>
+      <c r="C15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,C$12,$A$4,$A$5,$A$6,$A15,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3814124</v>
+      </c>
+      <c r="D15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,D$12,$A$4,$A$5,$A$6,$A15,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>1133805</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2011",0,"All Years\2011")</f>
+        <v>2011</v>
+      </c>
+      <c r="B16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,B$12,$A$4,$A$5,$A$6,$A16,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3884370</v>
+      </c>
+      <c r="C16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,C$12,$A$4,$A$5,$A$6,$A16,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3858049</v>
+      </c>
+      <c r="D16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,D$12,$A$4,$A$5,$A$6,$A16,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>1123577</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2012",0,"All Years\2012")</f>
+        <v>2012</v>
+      </c>
+      <c r="B17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,B$12,$A$4,$A$5,$A$6,$A17,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>656542</v>
+      </c>
+      <c r="C17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,C$12,$A$4,$A$5,$A$6,$A17,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>645577</v>
+      </c>
+      <c r="D17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,D$12,$A$4,$A$5,$A$6,$A17,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>192169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Stores","All Stores",1,"")</f>
+        <v>All Stores</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Designs","All Designs",1,"")</f>
+        <v>All Designs</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Facilities","Any Facilities",1,"")</f>
+        <v>Any Facilities</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"SalesPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PromotionalPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","All Years",1,"")</f>
+        <v>All Years</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Combos","All Combos",1,"")</f>
+        <v>All Combos</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Suppliers","All Suppliers",1,"")</f>
+        <v>All Suppliers</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$0 - $1.99",0,"All Prices\$0 - $1.99")</f>
+        <v>$0 - $1.99</v>
+      </c>
+      <c r="C12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$2 - $3.99",0,"All Prices\$2 - $3.99")</f>
+        <v>$2 - $3.99</v>
+      </c>
+      <c r="D12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$4 - $5.99",0,"All Prices\$4 - $5.99")</f>
+        <v>$4 - $5.99</v>
+      </c>
+      <c r="E12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$6 - $7.99",0,"All Prices\$6 - $7.99")</f>
+        <v>$6 - $7.99</v>
+      </c>
+      <c r="F12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$8 - $9.99",0,"All Prices\$8 - $9.99")</f>
+        <v>$8 - $9.99</v>
+      </c>
+      <c r="G12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$10+",0,"All Prices\$10+")</f>
+        <v>$10+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","0 - 249",0,"Any Calories\0 - 249")</f>
+        <v>0 - 249</v>
+      </c>
+      <c r="B13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A13)</f>
+        <v>39659</v>
+      </c>
+      <c r="C13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A13)</f>
+        <v>33262</v>
+      </c>
+      <c r="D13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A13)</f>
+        <v>267120</v>
+      </c>
+      <c r="E13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A13)</f>
+        <v>518321</v>
+      </c>
+      <c r="F13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A13)</f>
+        <v>250830</v>
+      </c>
+      <c r="G13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A13)</f>
+        <v>88012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","250 - 499",0,"Any Calories\250 - 499")</f>
+        <v>250 - 499</v>
+      </c>
+      <c r="B14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A14)</f>
+        <v>215156</v>
+      </c>
+      <c r="C14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A14)</f>
+        <v>542641</v>
+      </c>
+      <c r="D14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A14)</f>
+        <v>1174454</v>
+      </c>
+      <c r="E14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A14)</f>
+        <v>2285836</v>
+      </c>
+      <c r="F14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A14)</f>
+        <v>937573</v>
+      </c>
+      <c r="G14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A14)</f>
+        <v>736313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","500 - 749",0,"Any Calories\500 - 749")</f>
+        <v>500 - 749</v>
+      </c>
+      <c r="B15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A15)</f>
+        <v>196531</v>
+      </c>
+      <c r="C15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A15)</f>
+        <v>813815</v>
+      </c>
+      <c r="D15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A15)</f>
+        <v>1892577</v>
+      </c>
+      <c r="E15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A15)</f>
+        <v>2092180</v>
+      </c>
+      <c r="F15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A15)</f>
+        <v>1582964</v>
+      </c>
+      <c r="G15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A15)</f>
+        <v>465505</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","750 - 999",0,"Any Calories\750 - 999")</f>
+        <v>750 - 999</v>
+      </c>
+      <c r="B16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A16)</f>
+        <v>231538</v>
+      </c>
+      <c r="C16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A16)</f>
+        <v>1306629</v>
+      </c>
+      <c r="D16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A16)</f>
+        <v>2796125</v>
+      </c>
+      <c r="E16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A16)</f>
+        <v>2073792</v>
+      </c>
+      <c r="F16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A16)</f>
+        <v>1694113</v>
+      </c>
+      <c r="G16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A16)</f>
+        <v>683591</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","1000 - 1249",0,"Any Calories\1000 - 1249")</f>
+        <v>1000 - 1249</v>
+      </c>
+      <c r="B17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A17)</f>
+        <v>412256</v>
+      </c>
+      <c r="C17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A17)</f>
+        <v>1526286</v>
+      </c>
+      <c r="D17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A17)</f>
+        <v>1952059</v>
+      </c>
+      <c r="E17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A17)</f>
+        <v>1637293</v>
+      </c>
+      <c r="F17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A17)</f>
+        <v>1352035</v>
+      </c>
+      <c r="G17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A17)</f>
+        <v>720194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","1250 - 1499",0,"Any Calories\1250 - 1499")</f>
+        <v>1250 - 1499</v>
+      </c>
+      <c r="B18" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A18)</f>
+        <v>313283</v>
+      </c>
+      <c r="C18" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A18)</f>
+        <v>976590</v>
+      </c>
+      <c r="D18" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A18)</f>
+        <v>974022</v>
+      </c>
+      <c r="E18" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A18)</f>
+        <v>2053152</v>
+      </c>
+      <c r="F18" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A18)</f>
+        <v>1318660</v>
+      </c>
+      <c r="G18" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A18)</f>
+        <v>573930</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","1500+",0,"Any Calories\1500+")</f>
+        <v>1500+</v>
+      </c>
+      <c r="B19" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A19)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Stores","All Stores",1,"")</f>
+        <v>All Stores</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Designs","All Designs",1,"")</f>
+        <v>All Designs</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Facilities","Any Facilities",1,"")</f>
+        <v>Any Facilities</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"SalesPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PromotionalPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Combos","All Combos",1,"")</f>
+        <v>All Combos</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","All Prices",1,"")</f>
+        <v>All Prices</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","Any Calories",1,"")</f>
+        <v>Any Calories</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Suppliers","Greenham Suppliers Incorporated",0,"All Suppliers\Greenham Suppliers Incorporated")</f>
+        <v>Greenham Suppliers Incorporated</v>
+      </c>
+      <c r="C12" s="10" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Suppliers","Tyndall Wholefoods and Logistics Pty Ltd",0,"All Suppliers\Tyndall Wholefoods and Logistics Pty Ltd")</f>
+        <v>Tyndall Wholefoods and Logistics Pty Ltd</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2008",0,"All Years\2008")</f>
+        <v>2008</v>
+      </c>
+      <c r="B13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A13,$A$8,B$12,$A$9,$A$10)</f>
+        <v>4733528</v>
+      </c>
+      <c r="C13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A13,$A$8,C$12,$A$9,$A$10)</f>
+        <v>3887825</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2009",0,"All Years\2009")</f>
+        <v>2009</v>
+      </c>
+      <c r="B14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A14,$A$8,B$12,$A$9,$A$10)</f>
+        <v>3901927</v>
+      </c>
+      <c r="C14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A14,$A$8,C$12,$A$9,$A$10)</f>
+        <v>4990580</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2010",0,"All Years\2010")</f>
+        <v>2010</v>
+      </c>
+      <c r="B15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A15,$A$8,B$12,$A$9,$A$10)</f>
+        <v>4295970</v>
+      </c>
+      <c r="C15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A15,$A$8,C$12,$A$9,$A$10)</f>
+        <v>4558183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2011",0,"All Years\2011")</f>
+        <v>2011</v>
+      </c>
+      <c r="B16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A16,$A$8,B$12,$A$9,$A$10)</f>
+        <v>3784274</v>
+      </c>
+      <c r="C16" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A16,$A$8,C$12,$A$9,$A$10)</f>
+        <v>5081722</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","2012",0,"All Years\2012")</f>
+        <v>2012</v>
+      </c>
+      <c r="B17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A17,$A$8,B$12,$A$9,$A$10)</f>
+        <v>803812</v>
+      </c>
+      <c r="C17" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A17,$A$8,C$12,$A$9,$A$10)</f>
+        <v>690476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Designs","All Designs",1,"")</f>
+        <v>All Designs</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Facilities","Any Facilities",1,"")</f>
+        <v>Any Facilities</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PromotionalPeriods","All Periods",1,"")</f>
+        <v>All Periods</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Years","All Years",1,"")</f>
+        <v>All Years</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Combos","All Combos",1,"")</f>
+        <v>All Combos</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Suppliers","All Suppliers",1,"")</f>
+        <v>All Suppliers</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","All Prices",1,"")</f>
+        <v>All Prices</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","Any Calories",1,"")</f>
+        <v>Any Calories</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Stores","Australia",3,"All Stores\Australia")</f>
+        <v>Australia</v>
+      </c>
+      <c r="C12" s="13" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Stores","New Zealand",3,"All Stores\New Zealand")</f>
+        <v>New Zealand</v>
+      </c>
+      <c r="D12" s="13" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"Stores","Singapore",3,"All Stores\Singapore")</f>
+        <v>Singapore</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"SalesPeriods","Breakfast",0,"All Periods\Breakfast")</f>
+        <v>Breakfast</v>
+      </c>
+      <c r="B13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,B$12,$A$3,$A$4,$A13,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>2058098</v>
+      </c>
+      <c r="C13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,C$12,$A$3,$A$4,$A13,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>4912840</v>
+      </c>
+      <c r="D13" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,D$12,$A$3,$A$4,$A13,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>3695538</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"SalesPeriods","Lunch",0,"All Periods\Lunch")</f>
+        <v>Lunch</v>
+      </c>
+      <c r="B14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,B$12,$A$3,$A$4,$A14,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>6497830</v>
+      </c>
+      <c r="C14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,C$12,$A$3,$A$4,$A14,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>5978464</v>
+      </c>
+      <c r="D14" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,D$12,$A$3,$A$4,$A14,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>1675544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="str">
+        <f ca="1">_xll.PALO.ENAME($A$1,"SalesPeriods","Dinner",0,"All Periods\Dinner")</f>
+        <v>Dinner</v>
+      </c>
+      <c r="B15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,B$12,$A$3,$A$4,$A15,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>5020201</v>
+      </c>
+      <c r="C15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,C$12,$A$3,$A$4,$A15,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>2027055</v>
+      </c>
+      <c r="D15" s="12">
+        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,D$12,$A$3,$A$4,$A15,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
+        <v>4862727</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change per Aleck's specs
</commit_message>
<xml_diff>
--- a/Assignment1/data-import.xlsx
+++ b/Assignment1/data-import.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="345" windowWidth="28605" windowHeight="12630" activeTab="4"/>
+    <workbookView xWindow="-300" yWindow="345" windowWidth="28605" windowHeight="12630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1. Create Structure" sheetId="4" r:id="rId1"/>
     <sheet name="2. Create Data" sheetId="6" r:id="rId2"/>
     <sheet name="Facilities vs Years" sheetId="10" r:id="rId3"/>
     <sheet name="Designs vs Years" sheetId="11" r:id="rId4"/>
-    <sheet name="Price vs Calories" sheetId="12" r:id="rId5"/>
+    <sheet name="Price vs Calories" sheetId="16" r:id="rId5"/>
     <sheet name="Suppliers vs Years" sheetId="13" r:id="rId6"/>
     <sheet name="Country vs Sales Periods" sheetId="14" r:id="rId7"/>
   </sheets>
@@ -38,12 +38,12 @@
     <definedName name="_palopasteviewzerosuppressionalsocalculatednull" localSheetId="4">FALSE</definedName>
     <definedName name="_palopasteviewzerosuppressionalsocalculatednull" localSheetId="5">FALSE</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
   <si>
     <t>localhost/BurgerStore</t>
   </si>
@@ -213,24 +213,6 @@
     <t>PriceRange creation</t>
   </si>
   <si>
-    <t>$2 - $3.99</t>
-  </si>
-  <si>
-    <t>$0 - $1.99</t>
-  </si>
-  <si>
-    <t>$4 - $5.99</t>
-  </si>
-  <si>
-    <t>$6 - $7.99</t>
-  </si>
-  <si>
-    <t>$8 - $9.99</t>
-  </si>
-  <si>
-    <t>$10+</t>
-  </si>
-  <si>
     <t>← Make "All Prices"</t>
   </si>
   <si>
@@ -262,6 +244,15 @@
   </si>
   <si>
     <t>← Make "Any Calories"</t>
+  </si>
+  <si>
+    <t>$0 - $3.32</t>
+  </si>
+  <si>
+    <t>$3.33 - $6.65</t>
+  </si>
+  <si>
+    <t>$6.66+</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1351,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="L1" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1620,7 +1611,7 @@
     </row>
     <row r="18" spans="4:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G18" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$9,"c",$B$2,"All Stores",1)</f>
@@ -1760,103 +1751,73 @@
         <v>0</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="G29" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$17,"c","All Prices")</f>
         <v>0</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="4:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D30">
-        <v>200</v>
+        <v>333</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G30" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$29,"All Prices", 1)</f>
         <v>0</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="4:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D31">
-        <v>400</v>
+        <v>666</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="G31" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$30,"All Prices", 1)</f>
         <v>0</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="D32">
-        <v>600</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="E32" s="7"/>
       <c r="G32" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$31,"All Prices", 1)</f>
         <v>0</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="D33">
-        <v>800</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G33" s="5" t="b">
-        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$32,"All Prices", 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="E33" s="7"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="D34">
-        <v>1000</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G34" s="5" t="b">
-        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$33,"All Prices", 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="E34" s="7"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="4:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="G35" s="5" t="b">
-        <f ca="1">_xll.PALO.EADD($B$7,$D$17,"n",$E$34,"All Prices", 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>61</v>
-      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="4:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D36" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E36" s="7"/>
       <c r="G36" s="5"/>
@@ -1867,14 +1828,14 @@
         <v>0</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G37" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$18,"c","Any Calories")</f>
         <v>0</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1882,14 +1843,14 @@
         <v>250</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G38" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$37,"Any Calories", 1)</f>
         <v>0</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1897,14 +1858,14 @@
         <v>500</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G39" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$38,"Any Calories", 1)</f>
         <v>0</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1912,14 +1873,14 @@
         <v>750</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G40" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$39,"Any Calories", 1)</f>
         <v>0</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1927,14 +1888,14 @@
         <v>1000</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G41" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$40,"Any Calories", 1)</f>
         <v>0</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1942,14 +1903,14 @@
         <v>1250</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G42" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$41,"Any Calories", 1)</f>
         <v>0</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1957,14 +1918,14 @@
         <v>1500</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G43" s="5" t="b">
         <f ca="1">_xll.PALO.EADD($B$7,$D$18,"n",$E$42,"Any Calories", 1)</f>
         <v>0</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="4:8" ht="15" x14ac:dyDescent="0.25">
@@ -1973,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1986,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2068,7 +2029,7 @@
       </c>
       <c r="L2" s="1" t="str">
         <f>VLOOKUP($L$1,$D$29:$E$34,2,TRUE)</f>
-        <v>$0 - $1.99</v>
+        <v>$0 - $3.32</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>28</v>
@@ -2208,7 +2169,7 @@
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.2">
@@ -2279,52 +2240,37 @@
         <v>0</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30">
-        <v>200</v>
+        <v>333</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31">
-        <v>400</v>
+        <v>666</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D32">
-        <v>600</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D33">
-        <v>800</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D34">
-        <v>1000</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="E34" s="7"/>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E36" s="7"/>
     </row>
@@ -2333,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.2">
@@ -2341,7 +2287,7 @@
         <v>250</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.2">
@@ -2349,7 +2295,7 @@
         <v>500</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.2">
@@ -2357,7 +2303,7 @@
         <v>750</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.2">
@@ -2365,7 +2311,7 @@
         <v>1000</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.2">
@@ -2373,7 +2319,7 @@
         <v>1250</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.2">
@@ -2381,7 +2327,7 @@
         <v>1500</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2491,7 +2437,7 @@
       </c>
       <c r="D13" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,D$12,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
-        <v>2082676</v>
+        <v>2097224</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2668,7 +2614,7 @@
       </c>
       <c r="C13" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,C$12,$A$4,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
-        <v>3624583</v>
+        <v>3639131</v>
       </c>
       <c r="D13" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,D$12,$A$4,$A$5,$A$6,$A13,$A$7,$A$8,$A$9,$A$10)</f>
@@ -2754,103 +2700,89 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="14.7109375" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"Stores","All Stores",1,"")</f>
         <v>All Stores</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"Designs","All Designs",1,"")</f>
         <v>All Designs</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"Facilities","Any Facilities",1,"")</f>
         <v>Any Facilities</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"SalesPeriods","All Periods",1,"")</f>
         <v>All Periods</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"PromotionalPeriods","All Periods",1,"")</f>
         <v>All Periods</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"Years","All Years",1,"")</f>
         <v>All Years</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"Combos","All Combos",1,"")</f>
         <v>All Combos</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"Suppliers","All Suppliers",1,"")</f>
         <v>All Suppliers</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="str">
-        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$0 - $1.99",0,"All Prices\$0 - $1.99")</f>
-        <v>$0 - $1.99</v>
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$0 - $3.32",0,"All Prices\$0 - $3.32")</f>
+        <v>$0 - $3.32</v>
       </c>
       <c r="C12" s="10" t="str">
-        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$2 - $3.99",0,"All Prices\$2 - $3.99")</f>
-        <v>$2 - $3.99</v>
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$3.33 - $6.65",0,"All Prices\$3.33 - $6.65")</f>
+        <v>$3.33 - $6.65</v>
       </c>
       <c r="D12" s="10" t="str">
-        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$4 - $5.99",0,"All Prices\$4 - $5.99")</f>
-        <v>$4 - $5.99</v>
-      </c>
-      <c r="E12" s="10" t="str">
-        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$6 - $7.99",0,"All Prices\$6 - $7.99")</f>
-        <v>$6 - $7.99</v>
-      </c>
-      <c r="F12" s="10" t="str">
-        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$8 - $9.99",0,"All Prices\$8 - $9.99")</f>
-        <v>$8 - $9.99</v>
-      </c>
-      <c r="G12" s="10" t="str">
-        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$10+",0,"All Prices\$10+")</f>
-        <v>$10+</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <f ca="1">_xll.PALO.ENAME($A$1,"PriceRange","$6.66+",0,"All Prices\$6.66+")</f>
+        <v>$6.66+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","0 - 249",0,"Any Calories\0 - 249")</f>
         <v>0 - 249</v>
@@ -2861,176 +2793,104 @@
       </c>
       <c r="C13" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A13)</f>
-        <v>33262</v>
+        <v>502404</v>
       </c>
       <c r="D13" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A13)</f>
-        <v>267120</v>
-      </c>
-      <c r="E13" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A13)</f>
-        <v>518321</v>
-      </c>
-      <c r="F13" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A13)</f>
-        <v>250830</v>
-      </c>
-      <c r="G13" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A13)</f>
-        <v>88012</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>655141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","250 - 499",0,"Any Calories\250 - 499")</f>
         <v>250 - 499</v>
       </c>
       <c r="B14" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A14)</f>
-        <v>215156</v>
+        <v>471914</v>
       </c>
       <c r="C14" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A14)</f>
-        <v>542641</v>
+        <v>2225416</v>
       </c>
       <c r="D14" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A14)</f>
-        <v>1174454</v>
-      </c>
-      <c r="E14" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A14)</f>
-        <v>2285836</v>
-      </c>
-      <c r="F14" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A14)</f>
-        <v>937573</v>
-      </c>
-      <c r="G14" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A14)</f>
-        <v>736313</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>3194643</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","500 - 749",0,"Any Calories\500 - 749")</f>
         <v>500 - 749</v>
       </c>
       <c r="B15" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A15)</f>
-        <v>196531</v>
+        <v>693547</v>
       </c>
       <c r="C15" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A15)</f>
-        <v>813815</v>
+        <v>3133056</v>
       </c>
       <c r="D15" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A15)</f>
-        <v>1892577</v>
-      </c>
-      <c r="E15" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A15)</f>
-        <v>2092180</v>
-      </c>
-      <c r="F15" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A15)</f>
-        <v>1582964</v>
-      </c>
-      <c r="G15" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A15)</f>
-        <v>465505</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>3216969</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","750 - 999",0,"Any Calories\750 - 999")</f>
         <v>750 - 999</v>
       </c>
       <c r="B16" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A16)</f>
-        <v>231538</v>
+        <v>1085811</v>
       </c>
       <c r="C16" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A16)</f>
-        <v>1306629</v>
+        <v>4122365</v>
       </c>
       <c r="D16" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A16)</f>
-        <v>2796125</v>
-      </c>
-      <c r="E16" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A16)</f>
-        <v>2073792</v>
-      </c>
-      <c r="F16" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A16)</f>
-        <v>1694113</v>
-      </c>
-      <c r="G16" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A16)</f>
-        <v>683591</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>3577612</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","1000 - 1249",0,"Any Calories\1000 - 1249")</f>
         <v>1000 - 1249</v>
       </c>
       <c r="B17" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A17)</f>
-        <v>412256</v>
+        <v>1321554</v>
       </c>
       <c r="C17" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A17)</f>
-        <v>1526286</v>
+        <v>3293541</v>
       </c>
       <c r="D17" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A17)</f>
-        <v>1952059</v>
-      </c>
-      <c r="E17" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A17)</f>
-        <v>1637293</v>
-      </c>
-      <c r="F17" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A17)</f>
-        <v>1352035</v>
-      </c>
-      <c r="G17" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A17)</f>
-        <v>720194</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>2999576</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","1250 - 1499",0,"Any Calories\1250 - 1499")</f>
         <v>1250 - 1499</v>
       </c>
       <c r="B18" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,B$12,$A18)</f>
-        <v>313283</v>
+        <v>792149</v>
       </c>
       <c r="C18" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,C$12,$A18)</f>
-        <v>976590</v>
+        <v>2224614</v>
       </c>
       <c r="D18" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A18)</f>
-        <v>974022</v>
-      </c>
-      <c r="E18" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A18)</f>
-        <v>2053152</v>
-      </c>
-      <c r="F18" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A18)</f>
-        <v>1318660</v>
-      </c>
-      <c r="G18" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A18)</f>
-        <v>573930</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>3192874</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="str">
         <f ca="1">_xll.PALO.ENAME($A$1,"CalorieRange","1500+",0,"Any Calories\1500+")</f>
         <v>1500+</v>
@@ -3045,18 +2905,6 @@
       </c>
       <c r="D19" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,D$12,$A19)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,E$12,$A19)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,F$12,$A19)</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="12">
-        <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10,G$12,$A19)</f>
         <v>0</v>
       </c>
     </row>
@@ -3159,7 +3007,7 @@
       </c>
       <c r="C13" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,$A$3,$A$4,$A$5,$A$6,$A$7,$A13,$A$8,C$12,$A$9,$A$10)</f>
-        <v>3887825</v>
+        <v>3902373</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -3314,7 +3162,7 @@
       </c>
       <c r="B13" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,B$12,$A$3,$A$4,$A13,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>
-        <v>2058098</v>
+        <v>2072646</v>
       </c>
       <c r="C13" s="12">
         <f ca="1">_xll.PALO.DATAC($A$1,$A$2,C$12,$A$3,$A$4,$A13,$A$5,$A$6,$A$7,$A$8,$A$9,$A$10)</f>

</xml_diff>